<commit_message>
Load Screen code Updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>User_TC001</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>NO</t>
@@ -148,6 +145,26 @@
 f.) Search for edited record in AG grid
 g.) Click on delete button.
 h.) Check whether record exist in AG grid after delete.</t>
+  </si>
+  <si>
+    <t>Loads_TC003</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Validate whehter carrier user can add Scoular loads for payment using full submit
+1) Enter valid user id and Password and click Login button.
+2) Click on Add New Load button from Load menu.
+3) Enter valid details in all required field and click Save button
+4) Now loads are saved successfully.
+5) Upload an Origin and Destination ticket image or PDF document for corresponding load.
+6) Observe Ready to Submit Load icon in grid should change to green color.
+7) Click on Submit Load button.
+8) Select any option and click Submit button.</t>
+  </si>
+  <si>
+    <t>Scoular loads validated successfully</t>
   </si>
 </sst>
 </file>
@@ -218,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -228,6 +245,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,13 +580,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -574,116 +594,130 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
User Screen Code Updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>User_TC001</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>User_TC002</t>
   </si>
   <si>
@@ -49,34 +46,9 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Webtable validated successfully</t>
-  </si>
-  <si>
     <t>Invitation sent successfully</t>
   </si>
   <si>
-    <t>To validate invite via email based on following conditions
-1) Launch application and login as global admin
-2) Click on Users Menu
-3) Click on Add User button
-4) Enter valid details in required field (Full Name, Email)
-5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) 
-6) Select any one value from Carrier Drop Down field
-7) Click on Invite button and check invitation email sent successfully.
-8.) Clickon Resend Invitation and Check if invitation sent again.</t>
-  </si>
-  <si>
-    <t>To validate invite via email based on following conditions
-1) Launch application and login as global admin
-2) Click on Users Menu
-3) Click on Add User button
-4) Enter valid details in required field (Full Name, Email)
-5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) 
-6) Select any one value from Carrier Drop Down field
-7) Click on Invite button and check invitation email sent successfully.
-8.) Clickon cancel invitation and check if invitation cancelled.</t>
-  </si>
-  <si>
     <t>Invitation cancelled successfully</t>
   </si>
   <si>
@@ -86,36 +58,6 @@
     <t>User_TC003</t>
   </si>
   <si>
-    <t>To validate invite via email for Shipper Admin  based on following conditions
-1) Launch application and login as global admin
-2) Click on Users Menu
-3) Click on Add User button
-4) Enter valid details in required field (Full Name, Email)
-5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) 
-6) Select any one value from Carrier Drop Down field
-7) Click on Invite button and check invitation email sent successfully.
-8.) Accet email invitation and check if invitation acceted.</t>
-  </si>
-  <si>
-    <t>Validate whehter carrier user can add load and ready to submit load on following conditions
-1) Enter valid user id and Password and click Login button
-2) Click on Add New Load button from Load menu
-3) Enter valid details in all required field and click Save button
-4) Now loads are saved successfully
-5) Upload an Origin and Destination ticket image or PDF document for corresponding load
-6) Observe Ready to Submit Load icon in grid should change to green color
-7) Click on Submit Load button
-8) Select any option and click Submit button</t>
-  </si>
-  <si>
-    <t>Validate Forgot password based on following conditions:
-1. Launch application and Set UserName
-2. Clickon Forgot Password.
-3. Verify email and reset password
-4. Login with new password.
-5. Check whether user is able to login with new password.</t>
-  </si>
-  <si>
     <t>Password reset successfully</t>
   </si>
   <si>
@@ -125,32 +67,7 @@
     <t>User_TC005</t>
   </si>
   <si>
-    <t>Validate delete any user based on following conditions:
-1. Launch application 
-2. Login as global admin
-3. Go to Users and search accepted user(except global admin)
-4. Clickon delete
-5. Check whether deleted user exist.</t>
-  </si>
-  <si>
     <t>User deleted successfully</t>
-  </si>
-  <si>
-    <t>Validate whehter Global admin is able to add new load using Shipper platform on following conditions
-a.) Launch and login applcation as Global admin
-b.) Click on add new load button.
-C.) Set Carrier Name, Load Date, Shipper, Rate, Rate UOM and Commodity
-d.) click on save and search for record in AG grid.
-e.) click on Edit and set Shipper contact and click on save.
-f.) Search for edited record in AG grid
-g.) Click on delete button.
-h.) Check whether record exist in AG grid after delete.</t>
-  </si>
-  <si>
-    <t>Loads_TC003</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
   <si>
     <t>Validate whehter carrier user can add Scoular loads for payment using full submit
@@ -164,6 +81,81 @@
 8) Select any option and click Submit button.</t>
   </si>
   <si>
+    <t>To validate invite via email based on following conditions.
+1) Launch application and login as global admin.
+2) Click on Users Menu.
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions
+1) Launch application and login as global admin.
+2) Click on Users Menu.
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email)
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon cancel invitation and check if invitation cancelled.</t>
+  </si>
+  <si>
+    <t>To validate invite via email for Shipper Admin  based on following conditions
+1) Launch application and login as global admin.
+2) Click on Users Menu.
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email)
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Accet email invitation and check if invitation acceted.</t>
+  </si>
+  <si>
+    <t>Validate Forgot password based on following conditions:
+1. Launch application and Set UserName.
+2. Clickon Forgot Password.
+3. Verify email and reset password.
+4. Login with new password.
+5. Check whether user is able to login with new password.</t>
+  </si>
+  <si>
+    <t>Validate delete any  user based on following conditions:
+1. Launch application .
+2. Login as global admin.
+3. Go to Users and search accepted user(except global admin)
+4. Clickon delete.
+5. Check whether deleted user exist.</t>
+  </si>
+  <si>
+    <t>Validate whehter Global admin is able to add new load using Shipper platform on following conditions.
+a.) Launch and login applcation as Global admin
+b.) Click on add new load button.
+C.) Set Carrier Name, Load Date, Shipper, Rate, Rate UOM and Commodity.
+d.) click on save and search for record in AG grid.
+e.) click on Edit and set Shipper contact and click on save.
+f.) Search for edited record in AG grid
+g.) Click on delete button.
+h.) Check whether record exist in AG grid after delete.</t>
+  </si>
+  <si>
+    <t>Load submitted successfully</t>
+  </si>
+  <si>
+    <t>Load added successfully</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Loads_TC003</t>
+  </si>
+  <si>
     <t>Scoular loads validated successfully</t>
   </si>
   <si>
@@ -179,6 +171,9 @@
 6) Observe Ready to Submit Load icon in grid should change to green color.
 7) Click on Generate Invoice button.
 8) Select any option and click Generate button.</t>
+  </si>
+  <si>
+    <t>Webtable validated successfully</t>
   </si>
 </sst>
 </file>
@@ -568,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,13 +589,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -608,143 +603,129 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code for serial run issue
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -68,17 +68,6 @@
   </si>
   <si>
     <t>User deleted successfully</t>
-  </si>
-  <si>
-    <t>To validate invite via email based on following conditions.
-1) Launch application and login as global admin.
-2) Click on Users Menu.
-3) Click on Add User button.
-4) Enter valid details in required field (Full Name, Email).
-5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
-6) Select any one value from Carrier Drop Down field.
-7) Click on Invite button and check invitation email sent successfully.
-8.) Clickon Resend Invitation and Check if invitation sent again.</t>
   </si>
   <si>
     <t>To validate invite via email based on following conditions
@@ -119,17 +108,6 @@
 5. Check whether deleted user exist.</t>
   </si>
   <si>
-    <t>Validate whehter Global admin is able to add new load using Shipper platform on following conditions.
-a.) Launch and login applcation as Global admin
-b.) Click on add new load button.
-C.) Set Carrier Name, Load Date, Shipper, Rate, Rate UOM and Commodity.
-d.) click on save and search for record in AG grid.
-e.) click on Edit and set Shipper contact and click on save.
-f.) Search for edited record in AG grid
-g.) Click on delete button.
-h.) Check whether record exist in AG grid after delete.</t>
-  </si>
-  <si>
     <t>Load submitted successfully</t>
   </si>
   <si>
@@ -157,18 +135,6 @@
   </si>
   <si>
     <t>Non-Scoular Load Paid Successfully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate whehter carrier user can add Scoular loads for payment using full submit
-1) Enter valid user id and Password and click Login button.
-2) Click on Add New Load button from Load menu.
-3) Enter valid details in all required field and click Save button
-4) Now loads are saved successfully.
-5) Upload an Origin and Destination ticket image or PDF document for corresponding load.
-6) Observe Ready to Submit Load icon in grid should change to green color.
-7) Click on Submit Load button.
-8) Select any option and click Submit button.
-</t>
   </si>
   <si>
     <t>Validate whehter carrier user can add Scoular loads for payment using full submit.
@@ -194,6 +160,53 @@
   </si>
   <si>
     <t>Load Approved successfully</t>
+  </si>
+  <si>
+    <t>Loads_TC005</t>
+  </si>
+  <si>
+    <t>Dispatch sent successfully and carrier has control over load.</t>
+  </si>
+  <si>
+    <t>Validate whehter Global admin is able to add new load using Shipper platform on following conditions.
+a) Launch and login applcation as Global admin
+b) Click on add new load button.
+C) Set Carrier Name, Load Date, Shipper, Rate, Rate UOM and Commodity.
+d) click on save and search for record in AG grid.
+e) click on Edit and set Shipper contact and click on save.
+f) Search for edited record in AG grid
+g) Click on delete button.
+h) Check whether record exist in AG grid after delete.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate whehter carrier user can add Scoular loads for payment using full submit.
+1) Enter valid user id and Password and click Login button.
+2) Click on Add New Load button from Load menu.
+3) Enter valid details in all required field and click Save button
+4) Now loads are saved successfully.
+5) Upload an Origin and Destination ticket image or PDF document for corresponding load.
+6) Observe Ready to Submit Load icon in grid should change to green color.
+7) Click on Submit Load button.
+8) Select any option and click Submit button.
+</t>
+  </si>
+  <si>
+    <t>Validate the Dispatch Schedule loads to respective Carrier.
+1) Enter valid user id and Password and click Login button.
+2) Click on Add New Load button from Load menu.
+3) Enter valid details in required field and click Dispatch button.
+4) Now Loads are Dispatched to corresponding Carrier.</t>
+  </si>
+  <si>
+    <t>To validate invite via email based on following conditions.
+1) Launch application and login as global admin.
+2) Click on Users Menu and customize columns
+3) Click on Add User button.
+4) Enter valid details in required field (Full Name, Email).
+5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
+6) Select any one value from Carrier Drop Down field.
+7) Click on Invite button and check invitation email sent successfully.
+8.) Clickon Resend Invitation and Check if invitation sent again.</t>
   </si>
 </sst>
 </file>
@@ -583,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +636,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -637,10 +650,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -651,10 +664,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -665,10 +678,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -680,10 +693,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -695,13 +708,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -710,42 +723,56 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Code for Load
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -218,14 +218,6 @@
     <t>Validate the View PDF and Returned the load.
 1) Enter valid user id and Password and click Login button.
 2) Observe loads are displayed in Load grid.
-3) Select one or more loads and click Import button.
-4) Upload the excel sheet .
-5) Finish the load.</t>
-  </si>
-  <si>
-    <t>Validate the View PDF and Returned the load.
-1) Enter valid user id and Password and click Login button.
-2) Observe loads are displayed in Load grid.
 3) Select one or more loads and click view pdf button 1st download pdf then 2nd send via email.
 4) Login as Shipper Admin. 
 5) Select the Submitted Load.
@@ -299,6 +291,33 @@
   </si>
   <si>
     <t>Loads_TC008</t>
+  </si>
+  <si>
+    <t>Loads_TC009</t>
+  </si>
+  <si>
+    <t>Validate the Import File using Shipper Admin.
+1) Enter valid user id and Password and click Login button.
+2) Observe loads are displayed in Load grid.
+3) Select one or more loads and click Import button.
+4) Upload the excel sheet .
+5) Finish the load.</t>
+  </si>
+  <si>
+    <t>Validate the Import File using Global Admin.
+1) Enter valid user id and Password and click Login button.
+2) Observe loads are displayed in Load grid.
+3) Select one or more loads and click Import button.
+4) Upload the excel sheet .
+5) Finish the load.</t>
+  </si>
+  <si>
+    <t>Validate the Import File using Shipper User.
+1) Enter valid user id and Password and click Login button.
+2) Observe loads are displayed in Load grid.
+3) Select one or more loads and click Import button.
+4) Upload the excel sheet .
+5) Finish the load.</t>
   </si>
 </sst>
 </file>
@@ -444,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,7 +498,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -688,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +750,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -745,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -759,7 +778,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -773,7 +792,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -788,7 +807,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -797,13 +816,13 @@
     </row>
     <row r="7" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -812,13 +831,13 @@
     </row>
     <row r="8" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -827,13 +846,13 @@
     </row>
     <row r="9" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -842,13 +861,13 @@
     </row>
     <row r="10" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -863,7 +882,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -878,7 +897,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -893,7 +912,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -907,7 +926,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -921,7 +940,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -932,10 +951,10 @@
         <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -946,10 +965,10 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -957,15 +976,29 @@
     </row>
     <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Commit for Commodities
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -419,6 +419,46 @@
 c) Click on Change Password button.
 d) Fill Mandatory Details and click on Submit.
 e) Verify Newly change password by Re-Login.</t>
+  </si>
+  <si>
+    <t>AddCommodity_TC001</t>
+  </si>
+  <si>
+    <t>Validate whehter Global admin is able to add new Shipper on following conditions.
+a) Launch and login applcation as Global admin
+b) Goto commodities and Click on add new commodity button.
+C) Set Commodity name, upper limit, lower limit and pounds. 
+d) click on save.
+e) Customize Commodity webtable with required columns.
+f) Search for record and check if details dispalyed corrrect.
+g) Select record and click on delete button.
+h) check whether record deleted successfully.</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Commodity added and deleted successfully</t>
+  </si>
+  <si>
+    <t>EditCommodity_TC002</t>
+  </si>
+  <si>
+    <t>Validate whehter Global admin is able to add new Shipper on following conditions.
+a) Launch and login applcation as Global admin
+b) Goto commodities and Click on add new commodity button.
+C) Set Commodity name, upper limit, lower limit and pounds. 
+d) click on save.
+e) Customize Commodity webtable with required columns.
+f) Search for record and check if details dispalyed corrrect.
+g) Select record and edit with valid details.
+h) check whether record edited successfully.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Commodity added and edited successfully</t>
   </si>
 </sst>
 </file>
@@ -489,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,6 +543,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1157,7 @@
         <v>67</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>66</v>
@@ -1181,10 +1227,38 @@
         <v>73</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial Chat code Commit
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Automation Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -455,10 +455,16 @@
     <t>Commodity added and edited successfully</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Chat Validated successfully</t>
+  </si>
+  <si>
+    <t>Validate Chat</t>
+  </si>
+  <si>
+    <t>Chat_With_Carrier_TC001</t>
   </si>
 </sst>
 </file>
@@ -854,15 +860,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
@@ -1157,7 +1163,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>65</v>
@@ -1226,8 +1232,8 @@
       <c r="B25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>79</v>
+      <c r="C25" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>71</v>
@@ -1241,7 +1247,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>75</v>
@@ -1261,8 +1267,22 @@
         <v>78</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F27"/>
+  <autoFilter ref="A1:F28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Config and Test Data updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -890,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1317,7 +1317,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>80</v>
@@ -1331,7 +1331,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>80</v>
@@ -1345,7 +1345,7 @@
         <v>85</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Test Data and Config Updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1317,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>80</v>
@@ -1331,7 +1331,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>80</v>
@@ -1345,7 +1345,7 @@
         <v>85</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Field Mapping code Commit
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Automation Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$31</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -493,6 +493,24 @@
 17) Click on Send icon.
 18)Ensure document is displayed notification in Chat window for other chat person.
 19)Leave the chat</t>
+  </si>
+  <si>
+    <t>Load Validated Successfully</t>
+  </si>
+  <si>
+    <t>Field_Mapping_TC001</t>
+  </si>
+  <si>
+    <t>1) Enter valid user id and Password and click Login button in Scoular Shipper User.
+2) Click on Add New Load button.
+3) Enter valid details in required field.
+4) Select any value from drop down fields in Field Mapping at right hand side.
+5) Click on Save button.
+6) Select load and click Edit button.
+7) Enter valid details in required field.
+8) Select any value from drop down fields in Field Mapping at right hand side.
+9) Click on Save button.
+10)Select any Load and click Delete button.</t>
   </si>
 </sst>
 </file>
@@ -888,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1081,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1078,7 +1096,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1093,7 +1111,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1107,7 +1125,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -1121,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -1135,7 +1153,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1149,7 +1167,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1163,7 +1181,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1177,7 +1195,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1191,7 +1209,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>65</v>
@@ -1205,7 +1223,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>58</v>
@@ -1219,7 +1237,7 @@
         <v>60</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>61</v>
@@ -1233,7 +1251,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>64</v>
@@ -1247,7 +1265,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
@@ -1261,7 +1279,7 @@
         <v>72</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>71</v>
@@ -1275,7 +1293,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>75</v>
@@ -1289,7 +1307,7 @@
         <v>77</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>78</v>
@@ -1303,7 +1321,7 @@
         <v>85</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>80</v>
@@ -1317,7 +1335,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>80</v>
@@ -1331,7 +1349,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>80</v>
@@ -1345,14 +1363,28 @@
         <v>85</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F28"/>
+  <autoFilter ref="A1:F31"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Driver Test Case Updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -671,7 +671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,7 +706,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C11" sqref="C11:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1105,7 +1105,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1120,7 +1120,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1134,7 +1134,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -1148,7 +1148,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -1162,7 +1162,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1176,7 +1176,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1190,7 +1190,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1204,7 +1204,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1218,7 +1218,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>65</v>
@@ -1232,7 +1232,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>58</v>
@@ -1246,7 +1246,7 @@
         <v>60</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>61</v>
@@ -1260,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>64</v>
@@ -1274,7 +1274,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
@@ -1288,7 +1288,7 @@
         <v>72</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>71</v>
@@ -1302,7 +1302,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>75</v>
@@ -1316,7 +1316,7 @@
         <v>77</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>78</v>
@@ -1330,7 +1330,7 @@
         <v>85</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>80</v>
@@ -1344,7 +1344,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>80</v>
@@ -1358,7 +1358,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>80</v>
@@ -1372,7 +1372,7 @@
         <v>85</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>80</v>
@@ -1386,7 +1386,7 @@
         <v>88</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
         <v>86</v>
@@ -1400,7 +1400,7 @@
         <v>91</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Data and Config Updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1105,7 +1105,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1120,7 +1120,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1134,7 +1134,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -1148,7 +1148,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -1162,7 +1162,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1176,7 +1176,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1190,7 +1190,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1204,7 +1204,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1218,7 +1218,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>65</v>
@@ -1232,7 +1232,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>58</v>
@@ -1246,7 +1246,7 @@
         <v>60</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>61</v>
@@ -1260,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>64</v>
@@ -1274,7 +1274,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>67</v>
@@ -1288,7 +1288,7 @@
         <v>72</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>71</v>
@@ -1302,7 +1302,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>75</v>
@@ -1316,7 +1316,7 @@
         <v>77</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>78</v>
@@ -1330,7 +1330,7 @@
         <v>85</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>80</v>
@@ -1358,7 +1358,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>80</v>
@@ -1372,7 +1372,7 @@
         <v>85</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>80</v>
@@ -1400,7 +1400,7 @@
         <v>91</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
updated driver and config
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>Edit Load</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -915,7 +918,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C33"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +958,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -969,7 +972,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -983,7 +986,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -997,7 +1000,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1012,7 +1015,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1027,7 +1030,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1042,7 +1045,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1057,7 +1060,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -1072,7 +1075,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -1087,7 +1090,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1102,7 +1105,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1159,7 +1162,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1173,7 +1176,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1187,7 +1190,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1201,7 +1204,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1229,7 +1232,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
@@ -1243,7 +1246,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>60</v>
@@ -1271,7 +1274,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>66</v>
@@ -1285,7 +1288,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>70</v>
@@ -1299,7 +1302,7 @@
         <v>73</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>74</v>
@@ -1313,7 +1316,7 @@
         <v>76</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>77</v>
@@ -1383,7 +1386,7 @@
         <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
         <v>85</v>
@@ -1397,7 +1400,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
config and data updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -517,9 +517,6 @@
   </si>
   <si>
     <t>Edit Load</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -917,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +955,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -972,7 +969,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -986,7 +983,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -1000,7 +997,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1015,7 +1012,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1030,7 +1027,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1045,7 +1042,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1060,7 +1057,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -1075,7 +1072,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -1090,7 +1087,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1105,7 +1102,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1162,7 +1159,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1176,7 +1173,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1190,7 +1187,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1204,7 +1201,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1232,7 +1229,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
@@ -1246,7 +1243,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>60</v>
@@ -1274,7 +1271,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>66</v>
@@ -1288,7 +1285,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>70</v>
@@ -1302,7 +1299,7 @@
         <v>73</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>74</v>
@@ -1316,7 +1313,7 @@
         <v>76</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>77</v>
@@ -1386,7 +1383,7 @@
         <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
         <v>85</v>
@@ -1400,7 +1397,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Create Deal Code Update
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="6180"/>
@@ -10,14 +10,14 @@
     <sheet name="Automation Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$38</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -517,6 +517,74 @@
   </si>
   <si>
     <t>Edit Load</t>
+  </si>
+  <si>
+    <t>CreateDeal_TC001</t>
+  </si>
+  <si>
+    <t>Validate whehter Shipper user is able to add new Deal  on following conditions.
+a) Launch application and login applcation as Shipper admin
+b) Goto Deals and click on add icon
+c) Set mandatory fileds and clik on next.
+d.) Click on Deals and Drafts
+e.) Check whether the new deal widget added in Drafts</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CreateDeal_TC002</t>
+  </si>
+  <si>
+    <t>Validate whehter Shipper admin is able to add new Deal  on following conditions.
+a) Launch application and login applcation as Shipper user
+b) Goto Deals and click on add icon
+c) Set mandatory fileds and clik on next.
+d.) Click on Deals and Drafts
+e.) Check whether the new deal widget added in Drafts</t>
+  </si>
+  <si>
+    <t>CreateDeal_TC003</t>
+  </si>
+  <si>
+    <t>Validate whehter carrier is able to add new Deal  on following conditions.
+a) Launch application and login applcation as Shipper user
+b) Goto Deals and click on add icon
+c) Set mandatory fileds and clik on next.
+d.) Click on Deals and Drafts
+e.) Check whether the new deal widget added in Drafts</t>
+  </si>
+  <si>
+    <t>ShareDeal_TC001</t>
+  </si>
+  <si>
+    <t>Validate whehter Shipper user is able to share new Deal  on following conditions.
+a) Login with valid user id and Password 
+b) Click on Deals menu
+c) Click on Add New Deal button from Opportunity tab
+d) Select Dealname,EquipmentTypes &amp; # of Loads and click Next button
+e) Select one or more contacts(Carrier) in contact list screen and click share button
+f) Login as Carrier user and check opportunity tab whether Deal is displayed.</t>
+  </si>
+  <si>
+    <t>Deal has been shared</t>
+  </si>
+  <si>
+    <t>ShareDeal_TC002</t>
+  </si>
+  <si>
+    <t>Validate whehter Shipper admin is able to share all new Deal  on following conditions.
+a) Login withvalid user id and Password.
+b) Click on Deals menu
+c) Click on Add New Deal button from Opportunity tab
+d) Select Dealname,EquipmentTypes &amp; # of Loads and click Next button
+e) Goto Drafts and check Deal widget available.
+f) Select Deal, click on three dots and click on share.
+g) Set ON Share All and click Share.
+h) Login as Carrier user and check opportunity tab whether Deal is displayed.</t>
+  </si>
+  <si>
+    <t>Deal saved to draft</t>
   </si>
 </sst>
 </file>
@@ -668,7 +736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,7 +771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -912,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +1023,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -969,7 +1037,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -983,7 +1051,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -997,7 +1065,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1012,7 +1080,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1027,7 +1095,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1042,7 +1110,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1057,7 +1125,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -1072,7 +1140,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -1087,7 +1155,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1102,7 +1170,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1117,7 +1185,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
@@ -1131,7 +1199,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -1145,7 +1213,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>31</v>
@@ -1159,7 +1227,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
@@ -1173,7 +1241,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>39</v>
@@ -1187,7 +1255,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>39</v>
@@ -1201,7 +1269,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>39</v>
@@ -1215,7 +1283,7 @@
         <v>65</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>64</v>
@@ -1229,7 +1297,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
@@ -1243,7 +1311,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>60</v>
@@ -1257,7 +1325,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>63</v>
@@ -1271,7 +1339,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>66</v>
@@ -1285,7 +1353,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>70</v>
@@ -1299,7 +1367,7 @@
         <v>73</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>74</v>
@@ -1313,7 +1381,7 @@
         <v>76</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>77</v>
@@ -1327,7 +1395,7 @@
         <v>84</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>79</v>
@@ -1341,7 +1409,7 @@
         <v>84</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>79</v>
@@ -1355,7 +1423,7 @@
         <v>84</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>79</v>
@@ -1369,7 +1437,7 @@
         <v>84</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>79</v>
@@ -1383,7 +1451,7 @@
         <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
         <v>85</v>
@@ -1397,14 +1465,84 @@
         <v>90</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>89</v>
       </c>
     </row>
+    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F33"/>
+  <autoFilter ref="A1:F38"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
config mail & test case updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="173">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -853,9 +853,6 @@
   </si>
   <si>
     <t>Deal has been countered</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Deals_Chat_ShipperUser_TC001</t>
@@ -1374,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2134,7 @@
         <v>131</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>132</v>
@@ -2215,44 +2212,44 @@
     </row>
     <row r="59" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="C59" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="180" x14ac:dyDescent="0.25">
@@ -2263,7 +2260,7 @@
         <v>150</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>151</v>
@@ -2271,13 +2268,13 @@
     </row>
     <row r="63" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="C63" s="7" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>151</v>
@@ -2285,13 +2282,13 @@
     </row>
     <row r="64" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="C64" s="7" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>151</v>
@@ -2299,72 +2296,72 @@
     </row>
     <row r="65" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="C66" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="C67" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="C68" s="7" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="C69" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Config & Test cae updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:F80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,7 +2228,7 @@
         <v>117</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>118</v>
@@ -2644,7 +2644,7 @@
         <v>175</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>176</v>
@@ -2660,7 +2660,7 @@
         <v>175</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>176</v>
@@ -2788,7 +2788,7 @@
         <v>197</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Config & test data updated
</commit_message>
<xml_diff>
--- a/TestData/Driver.xlsx
+++ b/TestData/Driver.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="197">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -520,9 +520,6 @@
   </si>
   <si>
     <t>CreateDeal_TC001</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>CreateDeal_TC002</t>
@@ -1515,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1553,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -1572,7 +1569,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -1588,7 +1585,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -1604,7 +1601,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1620,7 +1617,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1636,7 +1633,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -1652,7 +1649,7 @@
         <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1668,7 +1665,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -1684,7 +1681,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -1700,7 +1697,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -1716,7 +1713,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1732,7 +1729,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>27</v>
@@ -1748,7 +1745,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -1764,7 +1761,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>31</v>
@@ -1780,7 +1777,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
@@ -1796,7 +1793,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>39</v>
@@ -1812,7 +1809,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>39</v>
@@ -1828,7 +1825,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>39</v>
@@ -1844,7 +1841,7 @@
         <v>65</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
@@ -1860,7 +1857,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>57</v>
@@ -1876,7 +1873,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>60</v>
@@ -1892,7 +1889,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>63</v>
@@ -1908,7 +1905,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>66</v>
@@ -1924,7 +1921,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>70</v>
@@ -1940,7 +1937,7 @@
         <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>74</v>
@@ -1956,7 +1953,7 @@
         <v>76</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>77</v>
@@ -1972,7 +1969,7 @@
         <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>79</v>
@@ -1988,7 +1985,7 @@
         <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>79</v>
@@ -2004,7 +2001,7 @@
         <v>84</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>79</v>
@@ -2020,7 +2017,7 @@
         <v>84</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>79</v>
@@ -2036,7 +2033,7 @@
         <v>87</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>85</v>
@@ -2052,7 +2049,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>89</v>
@@ -2065,733 +2062,733 @@
         <v>91</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="C46" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="C47" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="C49" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="C51" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="C52" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="C54" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="C55" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="C56" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C57" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="C58" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="C63" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="C64" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C66" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="C68" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="C69" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>178</v>
-      </c>
       <c r="C72" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="C74" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="C75" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="C77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="C78" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="C79" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="C80" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>